<commit_message>
Added loop to avg 10 samples
</commit_message>
<xml_diff>
--- a/Data/Plots_MI.xlsx
+++ b/Data/Plots_MI.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_Drive\Files\My Drive\Study_Stuff\Semester-8\Integrated_Laborotary_II\Experiment_1_LockInAmplifier_using_Expeyes\Codes_for_Expeyes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6606B868-560B-43FF-AE3B-C0EBFBD92B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73385B36-BFD4-4DDC-816C-4F3A850B06B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BB6EC1B-581E-4F94-A4A5-48A73DFECA37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6BB6EC1B-581E-4F94-A4A5-48A73DFECA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Avg" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>V_in (RMS)</t>
   </si>
@@ -56,12 +58,45 @@
   <si>
     <t>2000Hz</t>
   </si>
+  <si>
+    <t>200Hz</t>
+  </si>
+  <si>
+    <t>$V_{in}$</t>
+  </si>
+  <si>
+    <t>$V_{out}$</t>
+  </si>
+  <si>
+    <t>400Hz</t>
+  </si>
+  <si>
+    <t>800Hz</t>
+  </si>
+  <si>
+    <t>600Hz</t>
+  </si>
+  <si>
+    <t>800 Hz</t>
+  </si>
+  <si>
+    <t>200 Hz</t>
+  </si>
+  <si>
+    <t>400 Hz</t>
+  </si>
+  <si>
+    <t>600 Hz</t>
+  </si>
+  <si>
+    <t>1000 Hz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +107,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -108,6 +149,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1834,7 +1885,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9755383553330186E-2"/>
+          <c:y val="7.4843080697590103E-2"/>
+          <c:w val="0.79505225531861301"/>
+          <c:h val="0.89122986549570538"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1882,7 +1943,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$80:$D$92</c:f>
+              <c:f>Sheet1!$K$80:$K$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1930,7 +1991,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$80:$E$92</c:f>
+              <c:f>Sheet1!$L$80:$L$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2027,7 +2088,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$80:$B$92</c:f>
+              <c:f>Sheet1!$I$80:$I$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2075,7 +2136,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$80:$C$92</c:f>
+              <c:f>Sheet1!$J$80:$J$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2129,10 +2190,155 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>1500Hz</c:v>
+            <c:v>200Hz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$80:$G$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.35857714004927799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71557131476359204</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.07768572976111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4435441916495899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7958814636396201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1503978709576601</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5074077500553398</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8697613652696599</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2253992473067599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5846126585339699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9451275791154301</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.3073603130238602</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6652349742219199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$80:$H$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.8821298497651801E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8976837056012796E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4135008301956895E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3307508396152301E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.35247418252665E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.01722225308514E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.81268755493012E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1007294251730499E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.95858016340369E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8737176568553299E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5506288856664201E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5792935560703801E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.88165577451201E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-83FF-4C5B-BA45-5CE972E52E8A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>800Hz</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2156,265 +2362,28 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$80:$F$92</c:f>
+              <c:f>Sheet1!$M$80:$M$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0.359445476183333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.71687693293759502</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0792401994087299</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.44624697211586</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7971735390769601</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.1529670702880401</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5110765396260999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.8699799202744898</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.23036892483508</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.5888079666185702</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.9464758561122899</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.3065072124849202</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.6659018421057299</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$80:$G$92</c:f>
+              <c:f>Sheet1!$N$80:$N$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1.0599991715459201E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1731982065056098E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.3509411450040202E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.6007652143725498E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.9652839846429697E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.6618841634217596E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.08459533807523E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.14699068282785E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.2615749236703199E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2816586060977299E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3183141913595001E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.3432774458294799E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.32473252629521E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-4558-4BFE-A3C8-C90A7E655FA0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>2000Hz</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$80:$H$92</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0.35899007673759498</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.71711000787232004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0796569367593201</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4464660247421299</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7977136692926801</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.1533074837847801</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5106796526783302</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.86954454012159</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.2298357529700001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.5891221766325199</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.94675904024994</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.30779394080293</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.6653690255080003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$80:$I$92</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1.61201777836933E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.0333440603009504E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5249125260150299E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.8713929124859401E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.1789139424941698E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.9355050380691996E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0734626533338801E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.21834105510325E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.2537612681769001E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.26168377751454E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.29426129436736E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.3486313025350499E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.36352239735879E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-4558-4BFE-A3C8-C90A7E655FA0}"/>
+              <c16:uniqueId val="{00000009-83FF-4C5B-BA45-5CE972E52E8A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2636,6 +2605,1233 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>200Hz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$5:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.35857714004927799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71557131476359204</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.07768572976111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4435441916495899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7958814636396201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1503978709576601</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5074077500553398</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8697613652696599</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2253992473067599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5846126585339699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9451275791154301</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.3073603130238602</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6652349742219199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$5:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.8821298497651801E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8976837056012796E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4135008301956895E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3307508396152301E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.35247418252665E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.01722225308514E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.81268755493012E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1007294251730499E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.95858016340369E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8737176568553299E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5506288856664201E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5792935560703801E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.88165577451201E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2CD1-4F5B-8C31-6EF21768FCCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>400Hz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$5:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.35818855860587101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71689208763402201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.07919971034274</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.44551132866679</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7971165114572201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1530434158843801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.50868655798828</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8691076616983602</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.22686577771556</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.58643039240068</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.94182192380819</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.3047408811543004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6663902052128803</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$5:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.64308738245101E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9167951507223901E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.36504364995596E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.33272195240989E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1484365595860304E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0348690748415999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9592852369167804E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9277083804164599E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5979159580717896E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7964069439019501E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.96953378820344E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.7535655689017802E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.6329802502461503E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2CD1-4F5B-8C31-6EF21768FCCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>800Hz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$I$5:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.35890868471013798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71607138722395502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0789062448695901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.44637056500196</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7975325049056901</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1537803907648598</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.50821437655007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8710005288107499</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2306838730549501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5881750889733501</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9430335312406299</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.3087917419242903</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.66298515484986</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$5:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.9059332960018296E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.61228292905947E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8293464457871699E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0325234333091599E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1584170887390103E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9506546554856402E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7952633627823998E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5022513511187501E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9426774354887201E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8892739172549599E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.7784120238673501E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.9362947922410193E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.3804693794035995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2CD1-4F5B-8C31-6EF21768FCCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1121320655"/>
+        <c:axId val="1353759807"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1121320655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1353759807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1353759807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1121320655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>200 Hz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Avg!$C$5:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2.8694716815869499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.22834376930714</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5867199913921302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9455537659111801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3053019614361503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6645375206591098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0234203462546096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3840289831130903</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.7457533270102603</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1029207460116002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.4598473802401699</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.8243097211662702</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.1814726150642603</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Avg!$D$5:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.9200076689420201E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2902420277247599E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.41433171545371E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0682615156703901E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.90027729835257E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.90049494117179E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8107701690142401E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5470645619258699E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5465054392807998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.37994149415992E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8604837554989499E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.9494522307657099E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4890609573509398E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A1B3-4CD6-B8EE-A792FDD8419A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1256609999"/>
+        <c:axId val="1132676175"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>800 Hz</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Avg!$I$5:$I$18</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0">
+                        <c:v>0.35862858727445002</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.71680112160194498</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.0787385812930901</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.44571540360045</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.7969205329351701</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.1528977918458998</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.5101088321350198</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2.8686645052709401</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.22945503554448</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3.5878677920834399</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3.9463142935143001</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>4.3066764623158997</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4.6662961262162002</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>5.02342637412257</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Avg!$J$5:$J$18</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="14"/>
+                      <c:pt idx="0" formatCode="0.00E+00">
+                        <c:v>7.3907400746108494E-5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.52523377750626E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.63377117932686E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.9598540324953601E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3.82814176748083E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5.6729888697794697E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5.6600680460111802E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>9.4041627009890105E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9.5275468707860299E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8.9004367979597296E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>8.7242357567827999E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1.6838264870611399E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1.8833673537879999E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>2.84384588679708E-3</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-A1B3-4CD6-B8EE-A792FDD8419A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1256609999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1132676175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1132676175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1256609999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2716,6 +3912,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3233,6 +4509,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3788,16 +6096,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3817,6 +6125,88 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D1B329-4342-B106-3F4C-0A730F9726A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3E8457-B1DB-849D-65EE-741A9A870F6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4122,10 +6512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6D99D0-E2A0-4410-AB33-537FB9B2FC59}">
-  <dimension ref="B2:J92"/>
+  <dimension ref="B2:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79:H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5371,7 +7761,7 @@
         <v>4.5806103545365899E-3</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>1.9070395673460201</v>
       </c>
@@ -5385,7 +7775,7 @@
         <v>4.1766181651142703E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>1.94174113865063</v>
       </c>
@@ -5399,7 +7789,7 @@
         <v>4.9374316984851603E-3</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>1.9926661656089899</v>
       </c>
@@ -5413,7 +7803,7 @@
         <v>4.9468273878380204E-3</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>2.0586212717881498</v>
       </c>
@@ -5427,7 +7817,7 @@
         <v>4.7516008223423001E-3</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>2.1088911567743498</v>
       </c>
@@ -5441,7 +7831,7 @@
         <v>3.9603530577021102E-3</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>2.10898947964766</v>
       </c>
@@ -5449,374 +7839,1106 @@
         <v>2.2094536812884702E-3</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G78" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E79" s="3"/>
-      <c r="F79" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I79" s="3"/>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
+        <v>0.359445476183333</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1.0599991715459201E-3</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0.35899007673759498</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1.61201777836933E-4</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0.35857714004927799</v>
+      </c>
+      <c r="H80" s="1">
+        <v>1.8821298497651801E-4</v>
+      </c>
+      <c r="I80" s="1">
         <v>0.35915046736942802</v>
       </c>
-      <c r="C80" s="1">
+      <c r="J80" s="1">
         <v>3.28089070117295E-4</v>
       </c>
-      <c r="D80" s="1">
+      <c r="K80" s="1">
         <v>0.35839121544873198</v>
       </c>
-      <c r="E80" s="2">
+      <c r="L80" s="2">
         <v>8.96214070484862E-5</v>
       </c>
-      <c r="F80" s="1">
-        <v>0.359445476183333</v>
-      </c>
-      <c r="G80" s="1">
-        <v>1.0599991715459201E-3</v>
-      </c>
-      <c r="H80" s="1">
-        <v>0.35899007673759498</v>
-      </c>
-      <c r="I80" s="1">
-        <v>1.61201777836933E-4</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="1">
+        <v>0.71687693293759502</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2.1731982065056098E-3</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0.71711000787232004</v>
+      </c>
+      <c r="E81" s="1">
+        <v>6.0333440603009504E-4</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0.71557131476359204</v>
+      </c>
+      <c r="H81" s="1">
+        <v>4.8976837056012796E-4</v>
+      </c>
+      <c r="I81" s="1">
         <v>0.71690864353571304</v>
       </c>
-      <c r="C81" s="1">
+      <c r="J81" s="1">
         <v>6.3340701899839097E-4</v>
       </c>
-      <c r="D81" s="1">
+      <c r="K81" s="1">
         <v>0.71681740509139802</v>
       </c>
-      <c r="E81" s="1">
+      <c r="L81" s="1">
         <v>2.32585660823397E-4</v>
       </c>
-      <c r="F81" s="1">
-        <v>0.71687693293759502</v>
-      </c>
-      <c r="G81" s="1">
-        <v>2.1731982065056098E-3</v>
-      </c>
-      <c r="H81" s="1">
-        <v>0.71711000787232004</v>
-      </c>
-      <c r="I81" s="1">
-        <v>6.0333440603009504E-4</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
+        <v>1.0792401994087299</v>
+      </c>
+      <c r="C82" s="1">
+        <v>3.3509411450040202E-3</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1.0796569367593201</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1.5249125260150299E-3</v>
+      </c>
+      <c r="G82" s="1">
+        <v>1.07768572976111</v>
+      </c>
+      <c r="H82" s="1">
+        <v>9.4135008301956895E-4</v>
+      </c>
+      <c r="I82" s="1">
         <v>1.0794888657800701</v>
       </c>
-      <c r="C82" s="1">
+      <c r="J82" s="1">
         <v>7.7099095467998702E-4</v>
       </c>
-      <c r="D82" s="1">
+      <c r="K82" s="1">
         <v>1.0792491501049899</v>
       </c>
-      <c r="E82" s="1">
+      <c r="L82" s="1">
         <v>4.2388768265178798E-4</v>
       </c>
-      <c r="F82" s="1">
-        <v>1.0792401994087299</v>
-      </c>
-      <c r="G82" s="1">
-        <v>3.3509411450040202E-3</v>
-      </c>
-      <c r="H82" s="1">
-        <v>1.0796569367593201</v>
-      </c>
-      <c r="I82" s="1">
-        <v>1.5249125260150299E-3</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="1">
+        <v>1.44624697211586</v>
+      </c>
+      <c r="C83" s="1">
+        <v>5.6007652143725498E-3</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1.4464660247421299</v>
+      </c>
+      <c r="E83" s="1">
+        <v>2.8713929124859401E-3</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1.4435441916495899</v>
+      </c>
+      <c r="H83" s="1">
+        <v>1.3307508396152301E-3</v>
+      </c>
+      <c r="I83" s="1">
         <v>1.44656417988185</v>
       </c>
-      <c r="C83" s="1">
+      <c r="J83" s="1">
         <v>1.58863715732558E-3</v>
       </c>
-      <c r="D83" s="1">
+      <c r="K83" s="1">
         <v>1.4458662282799699</v>
       </c>
-      <c r="E83" s="1">
+      <c r="L83" s="1">
         <v>1.0036153310932501E-3</v>
       </c>
-      <c r="F83" s="1">
-        <v>1.44624697211586</v>
-      </c>
-      <c r="G83" s="1">
-        <v>5.6007652143725498E-3</v>
-      </c>
-      <c r="H83" s="1">
-        <v>1.4464660247421299</v>
-      </c>
-      <c r="I83" s="1">
-        <v>2.8713929124859401E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
+        <v>1.7971735390769601</v>
+      </c>
+      <c r="C84" s="1">
+        <v>6.9652839846429697E-3</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1.7977136692926801</v>
+      </c>
+      <c r="E84" s="1">
+        <v>4.1789139424941698E-3</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1.7958814636396201</v>
+      </c>
+      <c r="H84" s="1">
+        <v>1.35247418252665E-3</v>
+      </c>
+      <c r="I84" s="1">
         <v>1.7969522298949601</v>
       </c>
-      <c r="C84" s="1">
+      <c r="J84" s="1">
         <v>2.0109942581889098E-3</v>
       </c>
-      <c r="D84" s="1">
+      <c r="K84" s="1">
         <v>1.7965445446256301</v>
       </c>
-      <c r="E84" s="1">
+      <c r="L84" s="1">
         <v>1.7318760606739099E-3</v>
       </c>
-      <c r="F84" s="1">
-        <v>1.7971735390769601</v>
-      </c>
-      <c r="G84" s="1">
-        <v>6.9652839846429697E-3</v>
-      </c>
-      <c r="H84" s="1">
-        <v>1.7977136692926801</v>
-      </c>
-      <c r="I84" s="1">
-        <v>4.1789139424941698E-3</v>
-      </c>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
+        <v>2.1529670702880401</v>
+      </c>
+      <c r="C85" s="1">
+        <v>9.6618841634217596E-3</v>
+      </c>
+      <c r="D85" s="1">
+        <v>2.1533074837847801</v>
+      </c>
+      <c r="E85" s="1">
+        <v>9.9355050380691996E-3</v>
+      </c>
+      <c r="G85" s="1">
+        <v>2.1503978709576601</v>
+      </c>
+      <c r="H85" s="1">
+        <v>1.01722225308514E-3</v>
+      </c>
+      <c r="I85" s="1">
         <v>2.1528096528385601</v>
       </c>
-      <c r="C85" s="1">
+      <c r="J85" s="1">
         <v>1.2622396572866601E-3</v>
       </c>
-      <c r="D85" s="1">
+      <c r="K85" s="1">
         <v>2.1526406021018598</v>
       </c>
-      <c r="E85" s="1">
+      <c r="L85" s="1">
         <v>2.7554962562747099E-3</v>
       </c>
-      <c r="F85" s="1">
-        <v>2.1529670702880401</v>
-      </c>
-      <c r="G85" s="1">
-        <v>9.6618841634217596E-3</v>
-      </c>
-      <c r="H85" s="1">
-        <v>2.1533074837847801</v>
-      </c>
-      <c r="I85" s="1">
-        <v>9.9355050380691996E-3</v>
-      </c>
-    </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
+        <v>2.5110765396260999</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1.08459533807523E-2</v>
+      </c>
+      <c r="D86" s="1">
+        <v>2.5106796526783302</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1.0734626533338801E-2</v>
+      </c>
+      <c r="G86" s="1">
+        <v>2.5074077500553398</v>
+      </c>
+      <c r="H86" s="1">
+        <v>1.81268755493012E-3</v>
+      </c>
+      <c r="I86" s="1">
         <v>2.5112033907278901</v>
       </c>
-      <c r="C86" s="1">
+      <c r="J86" s="1">
         <v>2.0027827877799999E-3</v>
       </c>
-      <c r="D86" s="1">
+      <c r="K86" s="1">
         <v>2.5101009305505402</v>
       </c>
-      <c r="E86" s="1">
+      <c r="L86" s="1">
         <v>3.1553397608408001E-3</v>
       </c>
-      <c r="F86" s="1">
-        <v>2.5110765396260999</v>
-      </c>
-      <c r="G86" s="1">
-        <v>1.08459533807523E-2</v>
-      </c>
-      <c r="H86" s="1">
-        <v>2.5106796526783302</v>
-      </c>
-      <c r="I86" s="1">
-        <v>1.0734626533338801E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
+        <v>2.8699799202744898</v>
+      </c>
+      <c r="C87" s="1">
+        <v>1.14699068282785E-2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>2.86954454012159</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1.21834105510325E-2</v>
+      </c>
+      <c r="G87" s="1">
+        <v>2.8697613652696599</v>
+      </c>
+      <c r="H87" s="1">
+        <v>2.1007294251730499E-3</v>
+      </c>
+      <c r="I87" s="1">
         <v>2.8694010945897799</v>
       </c>
-      <c r="C87" s="1">
+      <c r="J87" s="1">
         <v>2.7784048704468101E-3</v>
       </c>
-      <c r="D87" s="1">
+      <c r="K87" s="1">
         <v>2.8688220349504698</v>
       </c>
-      <c r="E87" s="1">
+      <c r="L87" s="1">
         <v>5.0823984779949597E-3</v>
       </c>
-      <c r="F87" s="1">
-        <v>2.8699799202744898</v>
-      </c>
-      <c r="G87" s="1">
-        <v>1.14699068282785E-2</v>
-      </c>
-      <c r="H87" s="1">
-        <v>2.86954454012159</v>
-      </c>
-      <c r="I87" s="1">
-        <v>1.21834105510325E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
+        <v>3.23036892483508</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1.2615749236703199E-2</v>
+      </c>
+      <c r="D88" s="1">
+        <v>3.2298357529700001</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1.2537612681769001E-2</v>
+      </c>
+      <c r="G88" s="1">
+        <v>3.2253992473067599</v>
+      </c>
+      <c r="H88" s="1">
+        <v>1.95858016340369E-3</v>
+      </c>
+      <c r="I88" s="1">
         <v>3.2292919294910698</v>
       </c>
-      <c r="C88" s="1">
+      <c r="J88" s="1">
         <v>3.6260095433984299E-3</v>
       </c>
-      <c r="D88" s="1">
+      <c r="K88" s="1">
         <v>3.2291756326243002</v>
       </c>
-      <c r="E88" s="1">
+      <c r="L88" s="1">
         <v>4.1758335984973397E-3</v>
       </c>
-      <c r="F88" s="1">
-        <v>3.23036892483508</v>
-      </c>
-      <c r="G88" s="1">
-        <v>1.2615749236703199E-2</v>
-      </c>
-      <c r="H88" s="1">
-        <v>3.2298357529700001</v>
-      </c>
-      <c r="I88" s="1">
-        <v>1.2537612681769001E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
+        <v>3.5888079666185702</v>
+      </c>
+      <c r="C89" s="1">
+        <v>1.2816586060977299E-2</v>
+      </c>
+      <c r="D89" s="1">
+        <v>3.5891221766325199</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1.26168377751454E-2</v>
+      </c>
+      <c r="G89" s="1">
+        <v>3.5846126585339699</v>
+      </c>
+      <c r="H89" s="1">
+        <v>1.8737176568553299E-3</v>
+      </c>
+      <c r="I89" s="1">
         <v>3.5889629779859602</v>
       </c>
-      <c r="C89" s="1">
+      <c r="J89" s="1">
         <v>4.0615100103350002E-3</v>
       </c>
-      <c r="D89" s="1">
+      <c r="K89" s="1">
         <v>3.5884866289919799</v>
       </c>
-      <c r="E89" s="1">
+      <c r="L89" s="1">
         <v>6.0798393155930396E-3</v>
       </c>
-      <c r="F89" s="1">
-        <v>3.5888079666185702</v>
-      </c>
-      <c r="G89" s="1">
-        <v>1.2816586060977299E-2</v>
-      </c>
-      <c r="H89" s="1">
-        <v>3.5891221766325199</v>
-      </c>
-      <c r="I89" s="1">
-        <v>1.26168377751454E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" s="1">
+        <v>3.9464758561122899</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1.3183141913595001E-2</v>
+      </c>
+      <c r="D90" s="1">
+        <v>3.94675904024994</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1.29426129436736E-2</v>
+      </c>
+      <c r="G90" s="1">
+        <v>3.9451275791154301</v>
+      </c>
+      <c r="H90" s="1">
+        <v>3.5506288856664201E-3</v>
+      </c>
+      <c r="I90" s="1">
         <v>3.9463283545192702</v>
       </c>
-      <c r="C90" s="1">
+      <c r="J90" s="1">
         <v>4.9167489499808799E-3</v>
       </c>
-      <c r="D90" s="1">
+      <c r="K90" s="1">
         <v>3.9458508312362999</v>
       </c>
-      <c r="E90" s="1">
+      <c r="L90" s="1">
         <v>7.7174057367750499E-3</v>
       </c>
-      <c r="F90" s="1">
-        <v>3.9464758561122899</v>
-      </c>
-      <c r="G90" s="1">
-        <v>1.3183141913595001E-2</v>
-      </c>
-      <c r="H90" s="1">
-        <v>3.94675904024994</v>
-      </c>
-      <c r="I90" s="1">
-        <v>1.29426129436736E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
+        <v>4.3065072124849202</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1.3432774458294799E-2</v>
+      </c>
+      <c r="D91" s="1">
+        <v>4.30779394080293</v>
+      </c>
+      <c r="E91" s="1">
+        <v>1.3486313025350499E-2</v>
+      </c>
+      <c r="G91" s="1">
+        <v>4.3073603130238602</v>
+      </c>
+      <c r="H91" s="1">
+        <v>2.5792935560703801E-3</v>
+      </c>
+      <c r="I91" s="1">
         <v>4.3064166281061498</v>
       </c>
-      <c r="C91" s="1">
+      <c r="J91" s="1">
         <v>5.0820069184411999E-3</v>
       </c>
-      <c r="D91" s="1">
+      <c r="K91" s="1">
         <v>4.3070272029307803</v>
       </c>
-      <c r="E91" s="1">
+      <c r="L91" s="1">
         <v>9.6569402961264109E-3</v>
       </c>
-      <c r="F91" s="1">
-        <v>4.3065072124849202</v>
-      </c>
-      <c r="G91" s="1">
-        <v>1.3432774458294799E-2</v>
-      </c>
-      <c r="H91" s="1">
-        <v>4.30779394080293</v>
-      </c>
-      <c r="I91" s="1">
-        <v>1.3486313025350499E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
+        <v>4.6659018421057299</v>
+      </c>
+      <c r="C92" s="1">
+        <v>1.32473252629521E-2</v>
+      </c>
+      <c r="D92" s="1">
+        <v>4.6653690255080003</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1.36352239735879E-2</v>
+      </c>
+      <c r="G92" s="1">
+        <v>4.6652349742219199</v>
+      </c>
+      <c r="H92" s="1">
+        <v>2.88165577451201E-3</v>
+      </c>
+      <c r="I92" s="1">
         <v>4.6657028248456003</v>
       </c>
-      <c r="C92" s="1">
+      <c r="J92" s="1">
         <v>6.2106042803307896E-3</v>
       </c>
-      <c r="D92" s="1">
+      <c r="K92" s="1">
         <v>4.6645347084271496</v>
       </c>
-      <c r="E92" s="1">
+      <c r="L92" s="1">
         <v>9.3976015607955005E-3</v>
       </c>
-      <c r="F92" s="1">
-        <v>4.6659018421057299</v>
-      </c>
-      <c r="G92" s="1">
-        <v>1.32473252629521E-2</v>
-      </c>
-      <c r="H92" s="1">
-        <v>4.6653690255080003</v>
-      </c>
-      <c r="I92" s="1">
-        <v>1.36352239735879E-2</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K78:L78"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="B79:C79"/>
     <mergeCell ref="D79:E79"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="M78:N78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0396DC-9785-40BE-B4B5-796DE2097DB1}">
+  <dimension ref="C3:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="6">
+        <v>0.35857714004927799</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.8821298497651801E-4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.35818855860587101</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.64308738245101E-3</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
+        <v>0.35890868471013798</v>
+      </c>
+      <c r="J5" s="6">
+        <v>6.9059332960018296E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="6">
+        <v>0.71557131476359204</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4.8976837056012796E-4</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.71689208763402201</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1.9167951507223901E-3</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
+        <v>0.71607138722395502</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1.61228292905947E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="6">
+        <v>1.07768572976111</v>
+      </c>
+      <c r="D7" s="6">
+        <v>9.4135008301956895E-4</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.07919971034274</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2.36504364995596E-3</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6">
+        <v>1.0789062448695901</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1.8293464457871699E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="6">
+        <v>1.4435441916495899</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.3307508396152301E-3</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1.44551132866679</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3.33272195240989E-3</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>1.44637056500196</v>
+      </c>
+      <c r="J8" s="6">
+        <v>3.0325234333091599E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="6">
+        <v>1.7958814636396201</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.35247418252665E-3</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.7971165114572201</v>
+      </c>
+      <c r="F9" s="6">
+        <v>4.1484365595860304E-3</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
+        <v>1.7975325049056901</v>
+      </c>
+      <c r="J9" s="6">
+        <v>5.1584170887390103E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="6">
+        <v>2.1503978709576601</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.01722225308514E-3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2.1530434158843801</v>
+      </c>
+      <c r="F10" s="6">
+        <v>4.0348690748415999E-3</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <v>2.1537803907648598</v>
+      </c>
+      <c r="J10" s="6">
+        <v>4.9506546554856402E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="6">
+        <v>2.5074077500553398</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.81268755493012E-3</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2.50868655798828</v>
+      </c>
+      <c r="F11" s="6">
+        <v>4.9592852369167804E-3</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <v>2.50821437655007</v>
+      </c>
+      <c r="J11" s="6">
+        <v>6.7952633627823998E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="6">
+        <v>2.8697613652696599</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2.1007294251730499E-3</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2.8691076616983602</v>
+      </c>
+      <c r="F12" s="6">
+        <v>5.9277083804164599E-3</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <v>2.8710005288107499</v>
+      </c>
+      <c r="J12" s="6">
+        <v>5.5022513511187501E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="6">
+        <v>3.2253992473067599</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1.95858016340369E-3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3.22686577771556</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6.5979159580717896E-3</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
+        <v>3.2306838730549501</v>
+      </c>
+      <c r="J13" s="6">
+        <v>5.9426774354887201E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="6">
+        <v>3.5846126585339699</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.8737176568553299E-3</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3.58643039240068</v>
+      </c>
+      <c r="F14" s="6">
+        <v>4.7964069439019501E-3</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
+        <v>3.5881750889733501</v>
+      </c>
+      <c r="J14" s="6">
+        <v>6.8892739172549599E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="6">
+        <v>3.9451275791154301</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3.5506288856664201E-3</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3.94182192380819</v>
+      </c>
+      <c r="F15" s="6">
+        <v>4.96953378820344E-3</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6">
+        <v>3.9430335312406299</v>
+      </c>
+      <c r="J15" s="6">
+        <v>7.7784120238673501E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="6">
+        <v>4.3073603130238602</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2.5792935560703801E-3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>4.3047408811543004</v>
+      </c>
+      <c r="F16" s="6">
+        <v>4.7535655689017802E-3</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6">
+        <v>4.3087917419242903</v>
+      </c>
+      <c r="J16" s="6">
+        <v>7.9362947922410193E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="6">
+        <v>4.6652349742219199</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2.88165577451201E-3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4.6663902052128803</v>
+      </c>
+      <c r="F17" s="6">
+        <v>7.6329802502461503E-3</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6">
+        <v>4.66298515484986</v>
+      </c>
+      <c r="J17" s="6">
+        <v>9.3804693794035995E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21173FC7-759F-4281-B283-A64CF655C30B}">
+  <dimension ref="C3:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="3:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2.8694716815869499</v>
+      </c>
+      <c r="D5">
+        <v>1.9200076689420201E-4</v>
+      </c>
+      <c r="I5">
+        <v>0.35862858727445002</v>
+      </c>
+      <c r="J5" s="7">
+        <v>7.3907400746108494E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3.22834376930714</v>
+      </c>
+      <c r="D6">
+        <v>1.2902420277247599E-4</v>
+      </c>
+      <c r="I6">
+        <v>0.71680112160194498</v>
+      </c>
+      <c r="J6">
+        <v>1.52523377750626E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>3.5867199913921302</v>
+      </c>
+      <c r="D7">
+        <v>1.41433171545371E-3</v>
+      </c>
+      <c r="I7">
+        <v>1.0787385812930901</v>
+      </c>
+      <c r="J7">
+        <v>1.63377117932686E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3.9455537659111801</v>
+      </c>
+      <c r="D8">
+        <v>2.0682615156703901E-3</v>
+      </c>
+      <c r="I8">
+        <v>1.44571540360045</v>
+      </c>
+      <c r="J8">
+        <v>1.9598540324953601E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4.3053019614361503</v>
+      </c>
+      <c r="D9">
+        <v>1.90027729835257E-3</v>
+      </c>
+      <c r="I9">
+        <v>1.7969205329351701</v>
+      </c>
+      <c r="J9">
+        <v>3.82814176748083E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4.6645375206591098</v>
+      </c>
+      <c r="D10">
+        <v>1.90049494117179E-3</v>
+      </c>
+      <c r="I10">
+        <v>2.1528977918458998</v>
+      </c>
+      <c r="J10">
+        <v>5.6729888697794697E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>5.0234203462546096</v>
+      </c>
+      <c r="D11">
+        <v>1.8107701690142401E-3</v>
+      </c>
+      <c r="I11">
+        <v>2.5101088321350198</v>
+      </c>
+      <c r="J11">
+        <v>5.6600680460111802E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>5.3840289831130903</v>
+      </c>
+      <c r="D12">
+        <v>2.5470645619258699E-3</v>
+      </c>
+      <c r="I12">
+        <v>2.8686645052709401</v>
+      </c>
+      <c r="J12">
+        <v>9.4041627009890105E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>5.7457533270102603</v>
+      </c>
+      <c r="D13">
+        <v>2.5465054392807998E-3</v>
+      </c>
+      <c r="I13">
+        <v>3.22945503554448</v>
+      </c>
+      <c r="J13">
+        <v>9.5275468707860299E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>6.1029207460116002</v>
+      </c>
+      <c r="D14">
+        <v>2.37994149415992E-3</v>
+      </c>
+      <c r="I14">
+        <v>3.5878677920834399</v>
+      </c>
+      <c r="J14">
+        <v>8.9004367979597296E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>6.4598473802401699</v>
+      </c>
+      <c r="D15">
+        <v>2.8604837554989499E-3</v>
+      </c>
+      <c r="I15">
+        <v>3.9463142935143001</v>
+      </c>
+      <c r="J15">
+        <v>8.7242357567827999E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>6.8243097211662702</v>
+      </c>
+      <c r="D16">
+        <v>2.9494522307657099E-3</v>
+      </c>
+      <c r="I16">
+        <v>4.3066764623158997</v>
+      </c>
+      <c r="J16">
+        <v>1.6838264870611399E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>7.1814726150642603</v>
+      </c>
+      <c r="D17">
+        <v>3.4890609573509398E-3</v>
+      </c>
+      <c r="I17">
+        <v>4.6662961262162002</v>
+      </c>
+      <c r="J17">
+        <v>1.8833673537879999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>5.02342637412257</v>
+      </c>
+      <c r="J18">
+        <v>2.84384588679708E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>